<commit_message>
Adicionei o gráficos de gastos totais de Taubaté
</commit_message>
<xml_diff>
--- a/Dados/Dados de gastos/Taubate/gastos_saude2019-2022.xlsx
+++ b/Dados/Dados de gastos/Taubate/gastos_saude2019-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\API\dados de gastos\Taubate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120fd542a8b8b6a0/Área de Trabalho/API/Dados/Dados de gastos/Taubate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF84B11A-BB78-4A4A-833D-F2519B393E4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{CF84B11A-BB78-4A4A-833D-F2519B393E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06EF9CF9-D77A-433D-B76D-5EC6E47874E8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -269,7 +280,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15481714785651793"/>
+          <c:y val="0.17978006241729821"/>
+          <c:w val="0.81462729658792665"/>
+          <c:h val="0.58232201967324237"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -492,45 +513,67 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Anos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="916440671"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -559,7 +602,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="0"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Gasto em milhões (R$)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.6111111111111108E-2"/>
+              <c:y val="0.23358931524552243"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -593,6 +699,10 @@
         <c:crossAx val="916436511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="50000000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1521,20 +1631,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" s="7">
         <v>2019</v>
       </c>
@@ -1544,7 +1654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1559,7 +1669,7 @@
         <v>257988066.40000001</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1570,7 +1680,7 @@
         <v>251814459.06</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1581,14 +1691,14 @@
         <v>92625</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>2020</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1603,7 +1713,7 @@
         <v>291635372.81</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1614,7 +1724,7 @@
         <v>285943428.70999998</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1625,14 +1735,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>2021</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1757,7 @@
         <v>353708876.52000004</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1658,7 +1768,7 @@
         <v>347019017.85000002</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1669,14 +1779,14 @@
         <v>39279.57</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>2022</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1691,7 +1801,7 @@
         <v>424898237.37</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1702,7 +1812,7 @@
         <v>416602733.30000001</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1713,7 +1823,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D21" s="8">
         <f>SUM(D2:D19)</f>
         <v>1328230553.1000001</v>

</xml_diff>